<commit_message>
Project testing_project is saved. Author: user. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/testing_project/condition_error.xlsx
+++ b/DESIGN/rules/testing_project/condition_error.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\EPBDS-11702\openl-demo\user-workspace2\DEFAULT\fun666\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Steps</t>
   </si>
@@ -105,12 +105,22 @@
   </si>
   <si>
     <t>_res_</t>
+  </si>
+  <si>
+    <t>Datatype AllVa</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>sdsdsf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -169,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -227,11 +237,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -246,6 +274,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -560,7 +589,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7271BF-06A5-4BEC-9ED3-C856025AEA5C}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
@@ -568,83 +597,83 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26">
+      <c r="B26" s="0">
         <v>1</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="0">
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27">
+      <c r="B27" s="0">
         <v>2</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28">
+      <c r="B28" s="0">
         <v>3</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="0">
         <v>300</v>
       </c>
     </row>
@@ -774,9 +803,24 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
+    <row r="48">
+      <c r="B48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49">
+      <c r="B49" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s" s="8">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Project testing_project is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/testing_project/condition_error.xlsx
+++ b/DESIGN/rules/testing_project/condition_error.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>Steps</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>sdsdsf</t>
+  </si>
+  <si>
+    <t>vbnm</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
   <fonts count="5">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -179,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -255,11 +258,23 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -274,6 +289,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -589,7 +606,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7271BF-06A5-4BEC-9ED3-C856025AEA5C}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
@@ -810,15 +827,23 @@
       <c r="C48" s="8"/>
     </row>
     <row r="49">
-      <c r="B49" t="s" s="8">
+      <c r="B49" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C49" t="s" s="8">
+      <c r="C49" s="8" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="50">
+      <c r="B50" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B48:C48"/>
   </mergeCells>

</xml_diff>